<commit_message>
added password reset form
</commit_message>
<xml_diff>
--- a/src/lead/transactions.xlsx
+++ b/src/lead/transactions.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,30 +418,27 @@
         <v>leadStatus</v>
       </c>
       <c r="M1" t="str">
-        <v>followUp</v>
+        <v>organization</v>
       </c>
       <c r="N1" t="str">
-        <v>organization</v>
+        <v>campaign</v>
       </c>
       <c r="O1" t="str">
-        <v>campaign</v>
+        <v>nextAction</v>
       </c>
       <c r="P1" t="str">
-        <v>nextAction</v>
+        <v>type</v>
       </c>
       <c r="Q1" t="str">
-        <v>type</v>
-      </c>
-      <c r="R1" t="str">
         <v>__v</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>620c05c49c1c028850a00a2b</v>
+        <v>620ecb2be56ecb7e3608b811</v>
       </c>
       <c r="C2" t="str">
-        <v>2022-02-11T16:01:32.603Z</v>
+        <v>2022-02-16T21:34:17.553Z</v>
       </c>
       <c r="E2" t="str">
         <v>0</v>
@@ -450,48 +447,42 @@
         <v>0</v>
       </c>
       <c r="G2" t="str">
-        <v>6087bdfce55ce70702389085</v>
+        <v>60c3138a811f6b2197c8e3fa</v>
       </c>
       <c r="H2" t="str">
-        <v>mnsh0203@gmail.com</v>
+        <v>shanur.cse.nitap@gmail.com</v>
       </c>
       <c r="I2" t="str">
-        <v>mnsh0203@gmail.com</v>
+        <v>shanur.cse.nitap@gmail.com</v>
       </c>
       <c r="J2" t="str">
-        <v>Interested / warm to Interested / Hot by Manish</v>
+        <v>undefined to Not Interested / Already bought by shanur rahman</v>
       </c>
       <c r="K2" t="str">
-        <v>MR. AMIT  KUMAR  undefined</v>
+        <v>Anand Gupta undefined</v>
       </c>
       <c r="L2" t="str">
-        <v>Interested / Hot</v>
+        <v>Not Interested / Already bought</v>
       </c>
       <c r="M2" t="str">
-        <v>2022-02-15T20:07:53.488Z</v>
+        <v>5f663fcebb450386f9da5da8</v>
       </c>
       <c r="N2" t="str">
-        <v>5f663fcebb450386f9da5da8</v>
-      </c>
-      <c r="O2" t="str">
-        <v>6087bca57b7000001bd290a1</v>
-      </c>
-      <c r="P2" t="str">
-        <v>followUp</v>
+        <v>60c3133295e0dd001c9cc223</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
       </c>
       <c r="Q2">
-        <v>2</v>
-      </c>
-      <c r="R2">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>620ebbefe56ecb235b08b58d</v>
+        <v>621186fbe6d15809e86622e1</v>
       </c>
       <c r="C3" t="str">
-        <v>2022-02-16T21:34:17.553Z</v>
+        <v>2022-02-19T23:56:08.740Z</v>
       </c>
       <c r="E3" t="str">
         <v>0</v>
@@ -500,42 +491,39 @@
         <v>0</v>
       </c>
       <c r="G3" t="str">
-        <v>60c3138a811f6b2197c8e400</v>
+        <v>60c3138a811f6b2197c8e3fa</v>
       </c>
       <c r="H3" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
+        <v>mnsh0203@gmail.com</v>
       </c>
       <c r="I3" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Not Interested / Too Costly to Not Interested / Already bought by shanur rahman</v>
+        <v>mnsh0203@gmail.com</v>
       </c>
       <c r="K3" t="str">
-        <v>Dalip Singh undefined</v>
+        <v>Anand Gupta undefined</v>
       </c>
       <c r="L3" t="str">
         <v>Not Interested / Already bought</v>
       </c>
+      <c r="M3" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
       <c r="N3" t="str">
-        <v>5f663fcebb450386f9da5da8</v>
-      </c>
-      <c r="O3" t="str">
         <v>60c3133295e0dd001c9cc223</v>
       </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
       <c r="Q3">
-        <v>2</v>
-      </c>
-      <c r="R3">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>620ebd3ee56ecb218d08b603</v>
+        <v>621187881727184e6c2d360a</v>
       </c>
       <c r="C4" t="str">
-        <v>2022-02-16T21:34:17.553Z</v>
+        <v>2022-02-20T00:11:40.309Z</v>
       </c>
       <c r="E4" t="str">
         <v>0</v>
@@ -544,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="str">
-        <v>6084439e22dc72e3b27d0f22</v>
+        <v>60c3138a811f6b2197c8e3fa</v>
       </c>
       <c r="H4" t="str">
         <v>shanur.cse.nitap@gmail.com</v>
@@ -552,298 +540,28 @@
       <c r="I4" t="str">
         <v>shanur.cse.nitap@gmail.com</v>
       </c>
-      <c r="J4" t="str">
-        <v>testmanish to Callback by shanur rahman</v>
-      </c>
       <c r="K4" t="str">
-        <v>MR. ANUJ VERMA undefined</v>
+        <v>Anand Gupta undefined</v>
       </c>
       <c r="L4" t="str">
-        <v>Callback</v>
+        <v>Not Interested / Already bought</v>
+      </c>
+      <c r="M4" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
       </c>
       <c r="N4" t="str">
-        <v>5f663fcebb450386f9da5da8</v>
-      </c>
-      <c r="O4" t="str">
-        <v>608443356d59e1001b4fd388</v>
+        <v>60c3133295e0dd001c9cc223</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
       </c>
       <c r="Q4">
-        <v>2</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>620ecaace56ecbe27508b75b</v>
-      </c>
-      <c r="C5" t="str">
-        <v>2022-02-16T21:34:17.553Z</v>
-      </c>
-      <c r="E5" t="str">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="str">
-        <v>6084439e22dc72e3b27d0f22</v>
-      </c>
-      <c r="H5" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="I5" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="J5" t="str">
-        <v>Callback to testmanish by shanur rahman</v>
-      </c>
-      <c r="K5" t="str">
-        <v>MR. ANUJ VERMA undefined</v>
-      </c>
-      <c r="L5" t="str">
-        <v>testmanish</v>
-      </c>
-      <c r="N5" t="str">
-        <v>5f663fcebb450386f9da5da8</v>
-      </c>
-      <c r="O5" t="str">
-        <v>608443356d59e1001b4fd388</v>
-      </c>
-      <c r="Q5">
-        <v>2</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>620ecad3e56ecb548008b788</v>
-      </c>
-      <c r="C6" t="str">
-        <v>2022-02-16T21:34:17.553Z</v>
-      </c>
-      <c r="E6" t="str">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="str">
-        <v>60c3138a811f6b2197c8e428</v>
-      </c>
-      <c r="H6" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="I6" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="J6" t="str">
-        <v>undefined to Not Interested / Already bought by shanur rahman</v>
-      </c>
-      <c r="K6" t="str">
-        <v>Rajveer Saini undefined</v>
-      </c>
-      <c r="L6" t="str">
-        <v>Not Interested / Already bought</v>
-      </c>
-      <c r="N6" t="str">
-        <v>5f663fcebb450386f9da5da8</v>
-      </c>
-      <c r="O6" t="str">
-        <v>60c3133295e0dd001c9cc223</v>
-      </c>
-      <c r="P6" t="str">
-        <v>followUp</v>
-      </c>
-      <c r="Q6">
-        <v>2</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>620ecb2be56ecb7e3608b811</v>
-      </c>
-      <c r="C7" t="str">
-        <v>2022-02-16T21:34:17.553Z</v>
-      </c>
-      <c r="E7" t="str">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" t="str">
-        <v>60c3138a811f6b2197c8e3fa</v>
-      </c>
-      <c r="H7" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="I7" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="J7" t="str">
-        <v>undefined to Not Interested / Already bought by shanur rahman</v>
-      </c>
-      <c r="K7" t="str">
-        <v>Anand Gupta undefined</v>
-      </c>
-      <c r="L7" t="str">
-        <v>Not Interested / Already bought</v>
-      </c>
-      <c r="N7" t="str">
-        <v>5f663fcebb450386f9da5da8</v>
-      </c>
-      <c r="O7" t="str">
-        <v>60c3133295e0dd001c9cc223</v>
-      </c>
-      <c r="Q7">
-        <v>2</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>621186fbe6d15809e86622e1</v>
-      </c>
-      <c r="C8" t="str">
-        <v>2022-02-19T23:56:08.740Z</v>
-      </c>
-      <c r="E8" t="str">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" t="str">
-        <v>60c3138a811f6b2197c8e3fa</v>
-      </c>
-      <c r="H8" t="str">
-        <v>mnsh0203@gmail.com</v>
-      </c>
-      <c r="I8" t="str">
-        <v>mnsh0203@gmail.com</v>
-      </c>
-      <c r="K8" t="str">
-        <v>Anand Gupta undefined</v>
-      </c>
-      <c r="L8" t="str">
-        <v>Not Interested / Already bought</v>
-      </c>
-      <c r="N8" t="str">
-        <v>5f663fcebb450386f9da5da8</v>
-      </c>
-      <c r="O8" t="str">
-        <v>60c3133295e0dd001c9cc223</v>
-      </c>
-      <c r="Q8">
-        <v>2</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>621187881727184e6c2d360a</v>
-      </c>
-      <c r="C9" t="str">
-        <v>2022-02-20T00:11:40.309Z</v>
-      </c>
-      <c r="E9" t="str">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="str">
-        <v>60c3138a811f6b2197c8e3fa</v>
-      </c>
-      <c r="H9" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="I9" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="K9" t="str">
-        <v>Anand Gupta undefined</v>
-      </c>
-      <c r="L9" t="str">
-        <v>Not Interested / Already bought</v>
-      </c>
-      <c r="N9" t="str">
-        <v>5f663fcebb450386f9da5da8</v>
-      </c>
-      <c r="O9" t="str">
-        <v>60c3133295e0dd001c9cc223</v>
-      </c>
-      <c r="Q9">
-        <v>2</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>621d1cc71835f74a74d75daa</v>
-      </c>
-      <c r="C10" t="str">
-        <v>2022-02-28T17:27:49.378Z</v>
-      </c>
-      <c r="E10" t="str">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="str">
-        <v>60c3138a811f6b2197c8e400</v>
-      </c>
-      <c r="H10" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="I10" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="J10" t="str">
-        <v>Not Interested / Already bought to callback / followup by shanur rahman</v>
-      </c>
-      <c r="K10" t="str">
-        <v>Dalip Singh undefined</v>
-      </c>
-      <c r="L10" t="str">
-        <v>callback / followup</v>
-      </c>
-      <c r="M10" t="str">
-        <v>2022-03-01T19:04:34.420Z</v>
-      </c>
-      <c r="N10" t="str">
-        <v>5f663fcebb450386f9da5da8</v>
-      </c>
-      <c r="O10" t="str">
-        <v>60c3133295e0dd001c9cc223</v>
-      </c>
-      <c r="P10" t="str">
-        <v>followUp</v>
-      </c>
-      <c r="Q10">
-        <v>2</v>
-      </c>
-      <c r="R10">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:R10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added fullname to prospectname in lead history
</commit_message>
<xml_diff>
--- a/src/lead/transactions.xlsx
+++ b/src/lead/transactions.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,27 +418,33 @@
         <v>leadStatus</v>
       </c>
       <c r="M1" t="str">
+        <v>followUp</v>
+      </c>
+      <c r="N1" t="str">
         <v>organization</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>campaign</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>nextAction</v>
       </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
         <v>type</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>__v</v>
+      </c>
+      <c r="S1" t="str">
+        <v>campaignName</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>620ecb2be56ecb7e3608b811</v>
+        <v>620c05c49c1c028850a00a2b</v>
       </c>
       <c r="C2" t="str">
-        <v>2022-02-16T21:34:17.553Z</v>
+        <v>2022-02-11T16:01:32.603Z</v>
       </c>
       <c r="E2" t="str">
         <v>0</v>
@@ -447,42 +453,48 @@
         <v>0</v>
       </c>
       <c r="G2" t="str">
-        <v>60c3138a811f6b2197c8e3fa</v>
+        <v>6087bdfce55ce70702389085</v>
       </c>
       <c r="H2" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
+        <v>mnsh0203@gmail.com</v>
       </c>
       <c r="I2" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
+        <v>mnsh0203@gmail.com</v>
       </c>
       <c r="J2" t="str">
-        <v>undefined to Not Interested / Already bought by shanur rahman</v>
+        <v>Interested / warm to Interested / Hot by Manish</v>
       </c>
       <c r="K2" t="str">
-        <v>Anand Gupta undefined</v>
+        <v>MR. AMIT  KUMAR  undefined</v>
       </c>
       <c r="L2" t="str">
-        <v>Not Interested / Already bought</v>
+        <v>Interested / Hot</v>
       </c>
       <c r="M2" t="str">
-        <v>5f663fcebb450386f9da5da8</v>
+        <v>2022-02-15T20:07:53.488Z</v>
       </c>
       <c r="N2" t="str">
-        <v>60c3133295e0dd001c9cc223</v>
-      </c>
-      <c r="P2">
-        <v>2</v>
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O2" t="str">
+        <v>6087bca57b7000001bd290a1</v>
+      </c>
+      <c r="P2" t="str">
+        <v>followUp</v>
       </c>
       <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="R2">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>621186fbe6d15809e86622e1</v>
+        <v>620ebbefe56ecb235b08b58d</v>
       </c>
       <c r="C3" t="str">
-        <v>2022-02-19T23:56:08.740Z</v>
+        <v>2022-02-16T21:34:17.553Z</v>
       </c>
       <c r="E3" t="str">
         <v>0</v>
@@ -491,77 +503,728 @@
         <v>0</v>
       </c>
       <c r="G3" t="str">
-        <v>60c3138a811f6b2197c8e3fa</v>
+        <v>60c3138a811f6b2197c8e400</v>
       </c>
       <c r="H3" t="str">
-        <v>mnsh0203@gmail.com</v>
+        <v>shanur.cse.nitap@gmail.com</v>
       </c>
       <c r="I3" t="str">
-        <v>mnsh0203@gmail.com</v>
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Not Interested / Too Costly to Not Interested / Already bought by shanur rahman</v>
       </c>
       <c r="K3" t="str">
-        <v>Anand Gupta undefined</v>
+        <v>Dalip Singh undefined</v>
       </c>
       <c r="L3" t="str">
         <v>Not Interested / Already bought</v>
       </c>
-      <c r="M3" t="str">
-        <v>5f663fcebb450386f9da5da8</v>
-      </c>
       <c r="N3" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O3" t="str">
         <v>60c3133295e0dd001c9cc223</v>
       </c>
-      <c r="P3">
-        <v>2</v>
-      </c>
       <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
+        <v>620ebd3ee56ecb218d08b603</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2022-02-16T21:34:17.553Z</v>
+      </c>
+      <c r="E4" t="str">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="str">
+        <v>6084439e22dc72e3b27d0f22</v>
+      </c>
+      <c r="H4" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I4" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="J4" t="str">
+        <v>testmanish to Callback by shanur rahman</v>
+      </c>
+      <c r="K4" t="str">
+        <v>MR. ANUJ VERMA undefined</v>
+      </c>
+      <c r="L4" t="str">
+        <v>Callback</v>
+      </c>
+      <c r="N4" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O4" t="str">
+        <v>608443356d59e1001b4fd388</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>620ecaace56ecbe27508b75b</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2022-02-16T21:34:17.553Z</v>
+      </c>
+      <c r="E5" t="str">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="str">
+        <v>6084439e22dc72e3b27d0f22</v>
+      </c>
+      <c r="H5" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I5" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Callback to testmanish by shanur rahman</v>
+      </c>
+      <c r="K5" t="str">
+        <v>MR. ANUJ VERMA undefined</v>
+      </c>
+      <c r="L5" t="str">
+        <v>testmanish</v>
+      </c>
+      <c r="N5" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O5" t="str">
+        <v>608443356d59e1001b4fd388</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>620ecad3e56ecb548008b788</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2022-02-16T21:34:17.553Z</v>
+      </c>
+      <c r="E6" t="str">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="str">
+        <v>60c3138a811f6b2197c8e428</v>
+      </c>
+      <c r="H6" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I6" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="J6" t="str">
+        <v>undefined to Not Interested / Already bought by shanur rahman</v>
+      </c>
+      <c r="K6" t="str">
+        <v>Rajveer Saini undefined</v>
+      </c>
+      <c r="L6" t="str">
+        <v>Not Interested / Already bought</v>
+      </c>
+      <c r="N6" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O6" t="str">
+        <v>60c3133295e0dd001c9cc223</v>
+      </c>
+      <c r="P6" t="str">
+        <v>followUp</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>620ecb2be56ecb7e3608b811</v>
+      </c>
+      <c r="C7" t="str">
+        <v>2022-02-16T21:34:17.553Z</v>
+      </c>
+      <c r="E7" t="str">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="str">
+        <v>60c3138a811f6b2197c8e3fa</v>
+      </c>
+      <c r="H7" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I7" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="J7" t="str">
+        <v>undefined to Not Interested / Already bought by shanur rahman</v>
+      </c>
+      <c r="K7" t="str">
+        <v>Anand Gupta undefined</v>
+      </c>
+      <c r="L7" t="str">
+        <v>Not Interested / Already bought</v>
+      </c>
+      <c r="N7" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O7" t="str">
+        <v>60c3133295e0dd001c9cc223</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>621186fbe6d15809e86622e1</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2022-02-19T23:56:08.740Z</v>
+      </c>
+      <c r="E8" t="str">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="str">
+        <v>60c3138a811f6b2197c8e3fa</v>
+      </c>
+      <c r="H8" t="str">
+        <v>mnsh0203@gmail.com</v>
+      </c>
+      <c r="I8" t="str">
+        <v>mnsh0203@gmail.com</v>
+      </c>
+      <c r="K8" t="str">
+        <v>Anand Gupta undefined</v>
+      </c>
+      <c r="L8" t="str">
+        <v>Not Interested / Already bought</v>
+      </c>
+      <c r="N8" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O8" t="str">
+        <v>60c3133295e0dd001c9cc223</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
         <v>621187881727184e6c2d360a</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C9" t="str">
         <v>2022-02-20T00:11:40.309Z</v>
       </c>
-      <c r="E4" t="str">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="str">
+      <c r="E9" t="str">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="str">
         <v>60c3138a811f6b2197c8e3fa</v>
       </c>
-      <c r="H4" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="I4" t="str">
-        <v>shanur.cse.nitap@gmail.com</v>
-      </c>
-      <c r="K4" t="str">
+      <c r="H9" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I9" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="K9" t="str">
         <v>Anand Gupta undefined</v>
       </c>
-      <c r="L4" t="str">
+      <c r="L9" t="str">
         <v>Not Interested / Already bought</v>
       </c>
-      <c r="M4" t="str">
-        <v>5f663fcebb450386f9da5da8</v>
-      </c>
-      <c r="N4" t="str">
+      <c r="N9" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O9" t="str">
         <v>60c3133295e0dd001c9cc223</v>
       </c>
-      <c r="P4">
-        <v>2</v>
-      </c>
-      <c r="Q4">
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>621d1cc71835f74a74d75daa</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2022-02-28T17:27:49.378Z</v>
+      </c>
+      <c r="E10" t="str">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="str">
+        <v>60c3138a811f6b2197c8e400</v>
+      </c>
+      <c r="H10" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I10" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Not Interested / Already bought to callback / followup by shanur rahman</v>
+      </c>
+      <c r="K10" t="str">
+        <v>Dalip Singh undefined</v>
+      </c>
+      <c r="L10" t="str">
+        <v>callback / followup</v>
+      </c>
+      <c r="M10" t="str">
+        <v>2022-03-01T19:04:34.420Z</v>
+      </c>
+      <c r="N10" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O10" t="str">
+        <v>60c3133295e0dd001c9cc223</v>
+      </c>
+      <c r="P10" t="str">
+        <v>followUp</v>
+      </c>
+      <c r="Q10">
+        <v>2</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>6224321e7df61f3449ba4754</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2022-03-06T01:07:55.062Z</v>
+      </c>
+      <c r="E11" t="str">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="str">
+        <v>6084a433e55ce70702667995</v>
+      </c>
+      <c r="H11" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I11" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="J11" t="str">
+        <v>undefined to Not Interested / Already bought by shanur rahman</v>
+      </c>
+      <c r="K11" t="str">
+        <v>MRS. BHAGESHWARI DEVI undefined</v>
+      </c>
+      <c r="L11" t="str">
+        <v>Not Interested / Already bought</v>
+      </c>
+      <c r="N11" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O11" t="str">
+        <v>6083b5b06d59e1001b4fd2c6</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>6225365d7df61f794eba4873</v>
+      </c>
+      <c r="C12" t="str">
+        <v>2022-03-06T01:07:55.062Z</v>
+      </c>
+      <c r="E12" t="str">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="str">
+        <v>60c3138a811f6b2197c8e400</v>
+      </c>
+      <c r="H12" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I12" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="J12" t="str">
+        <v>callback / followup to Interested / warm by shanur rahman</v>
+      </c>
+      <c r="K12" t="str">
+        <v>Dalip Singh undefined</v>
+      </c>
+      <c r="L12" t="str">
+        <v>Interested / warm</v>
+      </c>
+      <c r="N12" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O12" t="str">
+        <v>60c3133295e0dd001c9cc223</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>622799df7df61f7c44ba4a5a</v>
+      </c>
+      <c r="C13" t="str">
+        <v>2022-03-06T01:07:55.062Z</v>
+      </c>
+      <c r="E13" t="str">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="str">
+        <v>6084a433e55ce707026678ff</v>
+      </c>
+      <c r="H13" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I13" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="J13" t="str">
+        <v>undefined to Interested / cold by shanur rahman</v>
+      </c>
+      <c r="K13" t="str">
+        <v>MR. AKHAND SINGH undefined</v>
+      </c>
+      <c r="L13" t="str">
+        <v>Interested / cold</v>
+      </c>
+      <c r="N13" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O13" t="str">
+        <v>6083b5b06d59e1001b4fd2c6</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>62279a347df61f1b27ba4a8a</v>
+      </c>
+      <c r="C14" t="str">
+        <v>2022-03-06T01:07:55.062Z</v>
+      </c>
+      <c r="E14" t="str">
+        <v/>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="str">
+        <v>60c3138a811f6b2197c8e400</v>
+      </c>
+      <c r="H14" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I14" t="str">
+        <v>mnsh0203@gmail.com</v>
+      </c>
+      <c r="J14" t="str">
+        <v>Lead reassigned from shanur.cse.nitap@gmail.com to mnsh0203@gmail.com by shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="N14" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O14" t="str">
+        <v>60c3133295e0dd001c9cc223</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14" t="str">
+        <v>Test Upload Campaign</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>62279a347df61f5300ba4a91</v>
+      </c>
+      <c r="C15" t="str">
+        <v>2022-03-06T01:07:55.062Z</v>
+      </c>
+      <c r="E15" t="str">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="str">
+        <v>60c3138a811f6b2197c8e400</v>
+      </c>
+      <c r="K15" t="str">
+        <v>Dalip Singh undefined</v>
+      </c>
+      <c r="L15" t="str">
+        <v>Interested / warm</v>
+      </c>
+      <c r="N15" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O15" t="str">
+        <v>60c3133295e0dd001c9cc223</v>
+      </c>
+      <c r="Q15">
+        <v>2</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>62254f9e90319213a49313ef</v>
+      </c>
+      <c r="C16" t="str">
+        <v>2022-03-07T00:13:57.231Z</v>
+      </c>
+      <c r="E16" t="str">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="str">
+        <v>6217b9bd7aecea279c22accf</v>
+      </c>
+      <c r="H16" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I16" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="J16" t="str">
+        <v>undefined to Interested / warm by shanur rahman</v>
+      </c>
+      <c r="K16" t="str">
+        <v>Undefined undefined</v>
+      </c>
+      <c r="L16" t="str">
+        <v>Interested / warm</v>
+      </c>
+      <c r="N16" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O16" t="str">
+        <v>6081c2cdc2fe0d001b7fa3b4</v>
+      </c>
+      <c r="Q16">
+        <v>2</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>6225503590319213a4931408</v>
+      </c>
+      <c r="C17" t="str">
+        <v>2022-03-07T00:13:57.231Z</v>
+      </c>
+      <c r="E17" t="str">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="str">
+        <v>6217bd99e30cf42d8c4bb059</v>
+      </c>
+      <c r="H17" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I17" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="J17" t="str">
+        <v>undefined to Interested / warm by shanur rahman</v>
+      </c>
+      <c r="K17" t="str">
+        <v>Undefined undefined</v>
+      </c>
+      <c r="L17" t="str">
+        <v>Interested / warm</v>
+      </c>
+      <c r="N17" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O17" t="str">
+        <v>6081c2cdc2fe0d001b7fa3b4</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>622551f8f974f61cc855a43c</v>
+      </c>
+      <c r="C18" t="str">
+        <v>2022-03-07T00:28:50.126Z</v>
+      </c>
+      <c r="E18" t="str">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="str">
+        <v>622535827df61f6a9aba4821</v>
+      </c>
+      <c r="H18" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I18" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="J18" t="str">
+        <v>undefined to Interested / Hot by shanur rahman</v>
+      </c>
+      <c r="K18" t="str">
+        <v>Undefined undefined</v>
+      </c>
+      <c r="L18" t="str">
+        <v>Interested / Hot</v>
+      </c>
+      <c r="N18" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O18" t="str">
+        <v>6081c2cdc2fe0d001b7fa3b4</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>6225523f70c3171f78ef5954</v>
+      </c>
+      <c r="C19" t="str">
+        <v>2022-03-07T00:30:48.044Z</v>
+      </c>
+      <c r="E19" t="str">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="str">
+        <v>622535827df61f6a9aba4821</v>
+      </c>
+      <c r="H19" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="I19" t="str">
+        <v>shanur.cse.nitap@gmail.com</v>
+      </c>
+      <c r="K19" t="str">
+        <v>Undefined undefined</v>
+      </c>
+      <c r="L19" t="str">
+        <v>Interested / Hot</v>
+      </c>
+      <c r="N19" t="str">
+        <v>5f663fcebb450386f9da5da8</v>
+      </c>
+      <c r="O19" t="str">
+        <v>6081c2cdc2fe0d001b7fa3b4</v>
+      </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:S19"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>